<commit_message>
Adición de notas corregidas.
</commit_message>
<xml_diff>
--- a/notasED/RubricaBenedettiGr51.xlsx
+++ b/notasED/RubricaBenedettiGr51.xlsx
@@ -148,7 +148,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,6 +197,14 @@
     <font>
       <u/>
       <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -407,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -473,6 +481,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,45 +550,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -891,66 +900,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -963,10 +972,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -1102,10 +1111,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -1127,11 +1136,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>14</v>
@@ -1160,10 +1169,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja11"/>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,66 +1184,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -1247,10 +1256,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -1281,7 +1290,7 @@
         <v>0.2</v>
       </c>
       <c r="D12" s="20">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
@@ -1294,7 +1303,9 @@
       <c r="C13" s="2">
         <v>0.1</v>
       </c>
-      <c r="D13" s="20"/>
+      <c r="D13" s="20">
+        <v>20</v>
+      </c>
     </row>
     <row r="14" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="17">
@@ -1306,7 +1317,9 @@
       <c r="C14" s="2">
         <v>0.05</v>
       </c>
-      <c r="D14" s="20"/>
+      <c r="D14" s="20">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="17">
@@ -1318,7 +1331,9 @@
       <c r="C15" s="2">
         <v>0.05</v>
       </c>
-      <c r="D15" s="20"/>
+      <c r="D15" s="20">
+        <v>20</v>
+      </c>
     </row>
     <row r="16" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="17">
@@ -1330,7 +1345,9 @@
       <c r="C16" s="2">
         <v>0.1</v>
       </c>
-      <c r="D16" s="20"/>
+      <c r="D16" s="20">
+        <v>20</v>
+      </c>
     </row>
     <row r="17" spans="1:4" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="17">
@@ -1342,7 +1359,9 @@
       <c r="C17" s="2">
         <v>0.2</v>
       </c>
-      <c r="D17" s="20"/>
+      <c r="D17" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="17">
@@ -1354,7 +1373,9 @@
       <c r="C18" s="2">
         <v>0.1</v>
       </c>
-      <c r="D18" s="20"/>
+      <c r="D18" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:4" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="17">
@@ -1366,13 +1387,15 @@
       <c r="C19" s="2">
         <v>0.1</v>
       </c>
-      <c r="D19" s="20"/>
+      <c r="D19" s="20">
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -1389,23 +1412,28 @@
       <c r="C21" s="2">
         <v>0.1</v>
       </c>
-      <c r="D21" s="18"/>
+      <c r="D21" s="18">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>35</v>
       </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1424,6 +1452,7 @@
     <mergeCell ref="A20:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1445,66 +1474,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -1517,10 +1546,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -1656,10 +1685,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -1681,11 +1710,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>11</v>
@@ -1729,66 +1758,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -1801,10 +1830,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -1940,10 +1969,10 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -1965,11 +1994,11 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>11</v>
@@ -2013,66 +2042,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -2085,10 +2114,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -2227,10 +2256,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -2252,11 +2281,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>17</v>
@@ -2300,66 +2329,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -2372,10 +2401,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -2514,10 +2543,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -2539,11 +2568,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>17</v>
@@ -2587,66 +2616,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -2659,10 +2688,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -2795,10 +2824,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -2823,11 +2852,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>15.5</v>
@@ -2872,66 +2901,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -2944,10 +2973,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -3083,10 +3112,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -3108,11 +3137,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>19.2</v>
@@ -3156,66 +3185,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -3228,10 +3257,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -3367,10 +3396,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -3395,11 +3424,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>15</v>
@@ -3443,66 +3472,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="42"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="32"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="23"/>
       <c r="B4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="32"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="48"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
@@ -3515,10 +3544,10 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="36" t="s">
+      <c r="A10" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="37"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="7" t="e">
         <f>SUM(C11,#REF!,C20)</f>
         <v>#REF!</v>
@@ -3654,10 +3683,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="38"/>
+      <c r="B20" s="51"/>
       <c r="C20" s="4">
         <f>C21</f>
         <v>0.1</v>
@@ -3682,11 +3711,11 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="6">
         <f>D12*0.2+D13*0.1+D14*0.05+D15*0.05+D16*0.1+D17*0.2+D18*0.1+D19*0.1+D21*0.1</f>
         <v>13</v>

</xml_diff>